<commit_message>
refactor: rm kafka and worker from CICD
</commit_message>
<xml_diff>
--- a/server-list.xlsx
+++ b/server-list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjingjie/Desktop/zwap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABEC37A-3203-1D44-B3A9-150280AAA7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB56627A-AB1F-094B-A7A4-C1D3527568B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="60" yWindow="780" windowWidth="34200" windowHeight="20380" xr2:uid="{F67A09E7-44DE-8E4A-BA87-B6ADD5082B8E}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="20300" xr2:uid="{F67A09E7-44DE-8E4A-BA87-B6ADD5082B8E}"/>
   </bookViews>
   <sheets>
     <sheet name="service" sheetId="1" r:id="rId1"/>
@@ -114,14 +114,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>curl -k -u elastic:'D_=V-k6LC8zXjpeTPk1V' https://linux-082:50005</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> kafka-console-consumer.sh   --bootstrap-server linux-085:50003   --topic mongo.test.test   --from-beginning   --property print.key=true   --property print.value=true</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Vault</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -210,6 +202,14 @@
   </si>
   <si>
     <t>vault status -address="http://127.0.0.1:50006" -token="hvs.YqRT7OysuTJxd2vC382IfiZK"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>curl -k -u elastic:'D_=V-k6LC8zXjpeTPk1V' http://linux-082:50005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kafka-console-consumer.sh --bootstrap-server linux-085:50003   --topic mongo.product.products   --from-beginning   --property print.key=true   --property print.value=true   --property key.separator=" | "</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -288,13 +288,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -634,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{881A6214-C266-AA48-A526-2F5D12C750A4}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -704,7 +704,7 @@
         <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -712,18 +712,18 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
         <v>22</v>
-      </c>
-      <c r="G6" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>23</v>
+      <c r="G7" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -731,23 +731,23 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>37</v>
+        <v>17</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="G10" s="2"/>
+      <c r="G10" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -766,68 +766,69 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScale="327" zoomScaleNormal="327" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
         <v>33</v>
-      </c>
-      <c r="B6" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
         <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: enhance error handling for connector configuration application in Jenkinsfile
</commit_message>
<xml_diff>
--- a/server-list.xlsx
+++ b/server-list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangjingjie/Desktop/zwap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB56627A-AB1F-094B-A7A4-C1D3527568B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804C3316-D75A-1549-9F04-E1B40B66001C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="20300" xr2:uid="{F67A09E7-44DE-8E4A-BA87-B6ADD5082B8E}"/>
+    <workbookView xWindow="-20" yWindow="780" windowWidth="34200" windowHeight="20300" xr2:uid="{F67A09E7-44DE-8E4A-BA87-B6ADD5082B8E}"/>
   </bookViews>
   <sheets>
     <sheet name="service" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>MongoDB</t>
   </si>
@@ -64,10 +64,6 @@
   <si>
     <t>Controller:linux-085.khoury.northeastern.edu:50004
 Listener: linux-085.khoury.northeastern.edu:50003</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>linux-084.khoury.northeastern.edu:50001</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -210,6 +206,18 @@
   </si>
   <si>
     <t>kafka-console-consumer.sh --bootstrap-server linux-085:50003   --topic mongo.product.products   --from-beginning   --property print.key=true   --property print.value=true   --property key.separator=" | "</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Schema registry</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>linux-083:50014</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>linux-084:50001</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -634,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{881A6214-C266-AA48-A526-2F5D12C750A4}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -654,10 +662,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
         <v>14</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -671,10 +679,10 @@
     </row>
     <row r="2" spans="1:8" ht="80">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="80">
@@ -683,7 +691,7 @@
       </c>
       <c r="C3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -698,55 +706,61 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
         <v>35</v>
       </c>
-      <c r="D9" t="s">
-        <v>36</v>
-      </c>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
       <c r="G10" s="4"/>
     </row>
   </sheetData>
@@ -777,58 +791,58 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
         <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
         <v>29</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>